<commit_message>
Agregados manejo de ficheros FileHandler.cpp y FileHandler.h ademas de un MAIN de prueba
</commit_message>
<xml_diff>
--- a/Seguimiento de Horas de trabajo.xlsx
+++ b/Seguimiento de Horas de trabajo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Día 1</t>
   </si>
@@ -542,10 +542,10 @@
                   <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -567,24 +567,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83371904"/>
-        <c:axId val="83373440"/>
+        <c:axId val="78505088"/>
+        <c:axId val="78506624"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="83371904"/>
+        <c:axId val="78505088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83373440"/>
+        <c:crossAx val="78506624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="83373440"/>
+        <c:axId val="78506624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83371904"/>
+        <c:crossAx val="78505088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -605,7 +605,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -809,25 +809,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83366272"/>
-        <c:axId val="83367808"/>
+        <c:axId val="82779520"/>
+        <c:axId val="82801792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83366272"/>
+        <c:axId val="82779520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83367808"/>
+        <c:crossAx val="82801792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83367808"/>
+        <c:axId val="82801792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +835,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83366272"/>
+        <c:crossAx val="82779520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -848,7 +848,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1174,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1185,7 +1185,7 @@
   <dimension ref="B2:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1319,11 +1319,11 @@
       </c>
       <c r="F5" s="17">
         <f t="shared" ref="F5:L5" si="0">SUM(F8:F16)</f>
-        <v>0</v>
+        <v>460</v>
       </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="H5" s="17">
         <f t="shared" si="0"/>
@@ -1485,16 +1485,18 @@
       <c r="E8" s="2">
         <v>60</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="3">
+        <v>60</v>
+      </c>
+      <c r="G8" s="4">
+        <v>60</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="5"/>
       <c r="K8" s="7"/>
       <c r="L8" s="6"/>
-      <c r="M8" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="M8" s="10"/>
       <c r="N8" s="5"/>
       <c r="O8" s="4"/>
       <c r="P8" s="5">
@@ -1553,16 +1555,18 @@
       <c r="E10" s="4">
         <v>80</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="2"/>
+      <c r="F10" s="3">
+        <v>120</v>
+      </c>
+      <c r="G10" s="2">
+        <v>45</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="K10" s="7"/>
       <c r="L10" s="6"/>
-      <c r="M10" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="M10" s="10"/>
       <c r="N10" s="5"/>
       <c r="O10" s="4"/>
       <c r="P10" s="5"/>
@@ -1585,16 +1589,18 @@
       <c r="E11" s="4">
         <v>80</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
+      <c r="F11" s="3">
+        <v>80</v>
+      </c>
+      <c r="G11" s="4">
+        <v>80</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="7"/>
       <c r="L11" s="6"/>
-      <c r="M11" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="M11" s="10"/>
       <c r="N11" s="5"/>
       <c r="O11" s="4"/>
       <c r="P11" s="5"/>
@@ -1617,16 +1623,18 @@
       <c r="E12" s="4">
         <v>80</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
+      <c r="F12" s="3">
+        <v>80</v>
+      </c>
+      <c r="G12" s="4">
+        <v>80</v>
+      </c>
       <c r="H12" s="5"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
       <c r="K12" s="7"/>
       <c r="L12" s="6"/>
-      <c r="M12" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="M12" s="10"/>
       <c r="N12" s="5"/>
       <c r="O12" s="4"/>
       <c r="P12" s="5"/>
@@ -1649,16 +1657,18 @@
       <c r="E13" s="4">
         <v>60</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="3">
+        <v>60</v>
+      </c>
+      <c r="G13" s="4">
+        <v>60</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
       <c r="K13" s="7"/>
       <c r="L13" s="6"/>
-      <c r="M13" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="M13" s="10"/>
       <c r="N13" s="5"/>
       <c r="O13" s="4"/>
       <c r="P13" s="5"/>
@@ -1741,16 +1751,18 @@
       <c r="E16" s="4">
         <v>60</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="3">
+        <v>60</v>
+      </c>
+      <c r="G16" s="4">
+        <v>60</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="4"/>
       <c r="J16" s="5"/>
       <c r="K16" s="7"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="10" t="s">
-        <v>20</v>
-      </c>
+      <c r="M16" s="10"/>
       <c r="N16" s="5"/>
       <c r="O16" s="4"/>
       <c r="P16" s="5"/>

</xml_diff>

<commit_message>
Subida Backlog, Sprint Backlogs y Segumiento
</commit_message>
<xml_diff>
--- a/Seguimiento de Horas de trabajo.xlsx
+++ b/Seguimiento de Horas de trabajo.xlsx
@@ -567,24 +567,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="78505088"/>
-        <c:axId val="78506624"/>
+        <c:axId val="74179712"/>
+        <c:axId val="74181248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="78505088"/>
+        <c:axId val="74179712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78506624"/>
+        <c:crossAx val="74181248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="78506624"/>
+        <c:axId val="74181248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78505088"/>
+        <c:crossAx val="74179712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -605,7 +605,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -809,25 +809,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82779520"/>
-        <c:axId val="82801792"/>
+        <c:axId val="74521984"/>
+        <c:axId val="74544256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82779520"/>
+        <c:axId val="74521984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82801792"/>
+        <c:crossAx val="74544256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82801792"/>
+        <c:axId val="74544256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +835,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82779520"/>
+        <c:crossAx val="74521984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -848,7 +848,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1174,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1185,7 +1185,7 @@
   <dimension ref="B2:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1561,7 +1561,9 @@
       <c r="G10" s="2">
         <v>45</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="K10" s="7"/>

</xml_diff>

<commit_message>
actualizado el seguimiento EXCEL
</commit_message>
<xml_diff>
--- a/Seguimiento de Horas de trabajo.xlsx
+++ b/Seguimiento de Horas de trabajo.xlsx
@@ -548,13 +548,13 @@
                   <c:v>385</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>340</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -567,24 +567,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74179712"/>
-        <c:axId val="74181248"/>
+        <c:axId val="81777792"/>
+        <c:axId val="81779328"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="74179712"/>
+        <c:axId val="81777792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74181248"/>
+        <c:crossAx val="81779328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="74181248"/>
+        <c:axId val="81779328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +592,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74179712"/>
+        <c:crossAx val="81777792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -605,7 +605,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -784,16 +784,16 @@
                   <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -809,25 +809,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74521984"/>
-        <c:axId val="74544256"/>
+        <c:axId val="83172736"/>
+        <c:axId val="83186816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74521984"/>
+        <c:axId val="83172736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74544256"/>
+        <c:crossAx val="83186816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74544256"/>
+        <c:axId val="83186816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +835,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74521984"/>
+        <c:crossAx val="83172736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -848,7 +848,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1174,7 +1174,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1184,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1327,15 +1327,15 @@
       </c>
       <c r="H5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="I5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="J5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="K5" s="17">
         <f t="shared" si="0"/>
@@ -1352,19 +1352,19 @@
       </c>
       <c r="O5" s="17">
         <f t="shared" ref="O5:U5" si="1">SUM(O8:O16)</f>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="P5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="R5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="S5" s="17">
         <f t="shared" si="1"/>
@@ -1491,10 +1491,18 @@
       <c r="G8" s="4">
         <v>60</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="7"/>
+      <c r="H8" s="5">
+        <v>60</v>
+      </c>
+      <c r="I8" s="4">
+        <v>60</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
       <c r="L8" s="6"/>
       <c r="M8" s="10"/>
       <c r="N8" s="5"/>
@@ -1564,9 +1572,15 @@
       <c r="H10" s="5">
         <v>0</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="7"/>
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
       <c r="L10" s="6"/>
       <c r="M10" s="10"/>
       <c r="N10" s="5"/>
@@ -1597,10 +1611,18 @@
       <c r="G11" s="4">
         <v>80</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="7"/>
+      <c r="H11" s="5">
+        <v>80</v>
+      </c>
+      <c r="I11" s="4">
+        <v>45</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
       <c r="L11" s="6"/>
       <c r="M11" s="10"/>
       <c r="N11" s="5"/>
@@ -1631,10 +1653,18 @@
       <c r="G12" s="4">
         <v>80</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="7"/>
+      <c r="H12" s="5">
+        <v>80</v>
+      </c>
+      <c r="I12" s="4">
+        <v>45</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
       <c r="L12" s="6"/>
       <c r="M12" s="10"/>
       <c r="N12" s="5"/>
@@ -1665,10 +1695,18 @@
       <c r="G13" s="4">
         <v>60</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="7"/>
+      <c r="H13" s="5">
+        <v>60</v>
+      </c>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
       <c r="L13" s="6"/>
       <c r="M13" s="10"/>
       <c r="N13" s="5"/>
@@ -1702,11 +1740,21 @@
       <c r="N14" s="5">
         <v>90</v>
       </c>
-      <c r="O14" s="4"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="4"/>
+      <c r="O14" s="4">
+        <v>90</v>
+      </c>
+      <c r="P14" s="5">
+        <v>90</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>90</v>
+      </c>
+      <c r="R14" s="5">
+        <v>45</v>
+      </c>
+      <c r="S14" s="4">
+        <v>0</v>
+      </c>
       <c r="T14" s="5"/>
       <c r="U14" s="6"/>
     </row>
@@ -1732,11 +1780,21 @@
       <c r="N15" s="5">
         <v>120</v>
       </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="4"/>
+      <c r="O15" s="4">
+        <v>120</v>
+      </c>
+      <c r="P15" s="5">
+        <v>120</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>120</v>
+      </c>
+      <c r="R15" s="5">
+        <v>30</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
       <c r="T15" s="5"/>
       <c r="U15" s="6"/>
     </row>
@@ -1759,10 +1817,18 @@
       <c r="G16" s="4">
         <v>60</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="7"/>
+      <c r="H16" s="5">
+        <v>60</v>
+      </c>
+      <c r="I16" s="4">
+        <v>60</v>
+      </c>
+      <c r="J16" s="5">
+        <v>60</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
       <c r="L16" s="6"/>
       <c r="M16" s="10"/>
       <c r="N16" s="5"/>

</xml_diff>

<commit_message>
Se ha añadido algunos métodos a ActivityHandler
</commit_message>
<xml_diff>
--- a/Seguimiento de Horas de trabajo.xlsx
+++ b/Seguimiento de Horas de trabajo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Día 1</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>Alex, Oscar</t>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
 </sst>
 </file>
@@ -557,34 +560,34 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81777792"/>
-        <c:axId val="81779328"/>
+        <c:axId val="67626112"/>
+        <c:axId val="67627648"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="81777792"/>
+        <c:axId val="67626112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81779328"/>
+        <c:crossAx val="67627648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="81779328"/>
+        <c:axId val="67627648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,7 +595,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81777792"/>
+        <c:crossAx val="67626112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -605,7 +608,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -693,21 +696,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$N$4:$U$4</c:f>
+              <c:f>Hoja1!$N$4:$T$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>210</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -716,9 +719,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -776,58 +776,55 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$N$5:$U$5</c:f>
+              <c:f>Hoja1!$N$5:$T$5</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>75</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83172736"/>
-        <c:axId val="83186816"/>
+        <c:axId val="69279104"/>
+        <c:axId val="69301376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83172736"/>
+        <c:axId val="69279104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="dd\-mmm" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83186816"/>
+        <c:crossAx val="69301376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83186816"/>
+        <c:axId val="69301376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +832,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83172736"/>
+        <c:crossAx val="69279104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -848,7 +845,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1185,7 +1182,7 @@
   <dimension ref="B2:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1284,16 +1281,16 @@
       </c>
       <c r="M4" s="13"/>
       <c r="N4" s="13">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="O4" s="13">
-        <v>110</v>
+        <v>180</v>
       </c>
       <c r="P4" s="13">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="Q4" s="13">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="R4" s="13">
         <v>0</v>
@@ -1339,44 +1336,44 @@
       </c>
       <c r="K5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="L5" s="17">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="17">
         <f>SUM(N8:N16)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="O5" s="17">
         <f t="shared" ref="O5:U5" si="1">SUM(O8:O16)</f>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="P5" s="17">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="Q5" s="17">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="R5" s="17">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="S5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="T5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="U5" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="2:21" ht="22.5" customHeight="1" thickTop="1" thickBot="1">
@@ -1387,27 +1384,51 @@
       <c r="E6" s="12">
         <v>6</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
+      <c r="F6" s="12">
+        <v>6</v>
+      </c>
+      <c r="G6" s="12">
+        <v>6</v>
+      </c>
+      <c r="H6" s="12">
+        <v>5</v>
+      </c>
+      <c r="I6" s="12">
+        <v>4</v>
+      </c>
+      <c r="J6" s="12">
+        <v>1</v>
+      </c>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
       <c r="L6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="12">
+        <v>3</v>
+      </c>
+      <c r="O6" s="12">
+        <v>3</v>
+      </c>
+      <c r="P6" s="12">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="12">
+        <v>3</v>
+      </c>
+      <c r="R6" s="12">
+        <v>3</v>
+      </c>
+      <c r="S6" s="12">
         <v>2</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
-      <c r="T6" s="12"/>
+      <c r="T6" s="12">
+        <v>2</v>
+      </c>
       <c r="U6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:21" ht="16.5" thickTop="1" thickBot="1">
@@ -1477,7 +1498,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>34</v>
@@ -1503,22 +1524,16 @@
       <c r="K8" s="7">
         <v>0</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
       <c r="M8" s="10"/>
       <c r="N8" s="5"/>
       <c r="O8" s="4"/>
-      <c r="P8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>0</v>
-      </c>
-      <c r="R8" s="5">
-        <v>0</v>
-      </c>
-      <c r="S8" s="4">
-        <v>0</v>
-      </c>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="4"/>
       <c r="T8" s="5"/>
       <c r="U8" s="6"/>
     </row>
@@ -1527,7 +1542,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>35</v>
@@ -1555,7 +1570,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>36</v>
@@ -1581,7 +1596,9 @@
       <c r="K10" s="7">
         <v>0</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="6">
+        <v>0</v>
+      </c>
       <c r="M10" s="10"/>
       <c r="N10" s="5"/>
       <c r="O10" s="4"/>
@@ -1597,7 +1614,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>20</v>
@@ -1623,7 +1640,9 @@
       <c r="K11" s="7">
         <v>0</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="6">
+        <v>0</v>
+      </c>
       <c r="M11" s="10"/>
       <c r="N11" s="5"/>
       <c r="O11" s="4"/>
@@ -1639,7 +1658,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>37</v>
@@ -1665,7 +1684,9 @@
       <c r="K12" s="7">
         <v>0</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="6">
+        <v>0</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="5"/>
       <c r="O12" s="4"/>
@@ -1681,7 +1702,7 @@
         <v>31</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>38</v>
@@ -1707,7 +1728,9 @@
       <c r="K13" s="7">
         <v>0</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="6">
+        <v>0</v>
+      </c>
       <c r="M13" s="10"/>
       <c r="N13" s="5"/>
       <c r="O13" s="4"/>
@@ -1723,7 +1746,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="4"/>
@@ -1735,28 +1758,32 @@
       <c r="K14" s="7"/>
       <c r="L14" s="6"/>
       <c r="M14" s="10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="N14" s="5">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="O14" s="4">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="P14" s="5">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="Q14" s="4">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="R14" s="5">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="S14" s="4">
         <v>0</v>
       </c>
-      <c r="T14" s="5"/>
-      <c r="U14" s="6"/>
+      <c r="T14" s="5">
+        <v>0</v>
+      </c>
+      <c r="U14" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:21">
       <c r="B15" s="16" t="s">
@@ -1775,7 +1802,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="6"/>
       <c r="M15" s="10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="N15" s="5">
         <v>120</v>
@@ -1790,13 +1817,17 @@
         <v>120</v>
       </c>
       <c r="R15" s="5">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="S15" s="4">
-        <v>0</v>
-      </c>
-      <c r="T15" s="5"/>
-      <c r="U15" s="6"/>
+        <v>120</v>
+      </c>
+      <c r="T15" s="5">
+        <v>120</v>
+      </c>
+      <c r="U15" s="6">
+        <v>120</v>
+      </c>
     </row>
     <row r="16" spans="2:21">
       <c r="B16" s="16" t="s">
@@ -1827,18 +1858,38 @@
         <v>60</v>
       </c>
       <c r="K16" s="7">
-        <v>0</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="L16" s="6">
+        <v>60</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N16" s="5">
+        <v>60</v>
+      </c>
+      <c r="O16" s="4">
+        <v>60</v>
+      </c>
+      <c r="P16" s="5">
+        <v>60</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>60</v>
+      </c>
+      <c r="R16" s="5">
+        <v>60</v>
+      </c>
+      <c r="S16" s="4">
+        <v>60</v>
+      </c>
+      <c r="T16" s="5">
+        <v>60</v>
+      </c>
+      <c r="U16" s="6">
+        <v>60</v>
+      </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17"/>

</xml_diff>